<commit_message>
Adicionado Imagens de tutorial do app
</commit_message>
<xml_diff>
--- a/Estoque_Games.xlsx
+++ b/Estoque_Games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Marca</t>
   </si>
@@ -31,25 +31,28 @@
     <t>Capa</t>
   </si>
   <si>
-    <t>afd</t>
-  </si>
-  <si>
-    <t>ada</t>
-  </si>
-  <si>
-    <t>dfdfd</t>
+    <t>Rockstar</t>
+  </si>
+  <si>
+    <t>Mojang</t>
   </si>
   <si>
     <t>GTA V</t>
   </si>
   <si>
-    <t>fdfd</t>
+    <t>Red Dead Redemption II</t>
+  </si>
+  <si>
+    <t>Minecraft</t>
+  </si>
+  <si>
+    <t>PC</t>
   </si>
   <si>
     <t>PS4</t>
   </si>
   <si>
-    <t>?</t>
+    <t>Xbox 360</t>
   </si>
 </sst>
 </file>
@@ -131,13 +134,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>1752600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -155,8 +158,84 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
+          <a:off x="6429375" y="438150"/>
+          <a:ext cx="1143000" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1600200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Red Dead Redemption II.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
           <a:off x="6429375" y="2343150"/>
-          <a:ext cx="1143000" cy="1562100"/>
+          <a:ext cx="1143000" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1552575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Minecraft.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6429375" y="4248150"/>
+          <a:ext cx="1143000" cy="1362075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -453,7 +532,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -492,13 +571,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="150" customHeight="1">
@@ -506,16 +582,33 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1">
-        <v>10</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="150" customHeight="1">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aplicativo atualizado para utilizar requests
</commit_message>
<xml_diff>
--- a/Estoque_Games.xlsx
+++ b/Estoque_Games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Marca</t>
   </si>
@@ -34,25 +34,46 @@
     <t>Rockstar</t>
   </si>
   <si>
+    <t>dada</t>
+  </si>
+  <si>
     <t>Mojang</t>
   </si>
   <si>
+    <t>Activision</t>
+  </si>
+  <si>
     <t>GTA V</t>
   </si>
   <si>
-    <t>Red Dead Redemption II</t>
+    <t>Need For Speed</t>
+  </si>
+  <si>
+    <t>fdfd</t>
   </si>
   <si>
     <t>Minecraft</t>
   </si>
   <si>
+    <t>Black Ops II</t>
+  </si>
+  <si>
+    <t>Xbox One</t>
+  </si>
+  <si>
+    <t>PS4</t>
+  </si>
+  <si>
+    <t>dfd</t>
+  </si>
+  <si>
     <t>PC</t>
   </si>
   <si>
-    <t>PS4</t>
-  </si>
-  <si>
     <t>Xbox 360</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -179,11 +200,11 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>1600200</xdr:rowOff>
+      <xdr:rowOff>1552575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="Red Dead Redemption II.jpg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Need For Speed.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -197,7 +218,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6429375" y="2343150"/>
-          <a:ext cx="1143000" cy="1409700"/>
+          <a:ext cx="1143000" cy="1362075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -210,13 +231,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>1552575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -234,8 +255,46 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6429375" y="4248150"/>
+          <a:off x="6429375" y="6153150"/>
           <a:ext cx="1143000" cy="1362075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1600200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Black Ops II.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6429375" y="8058150"/>
+          <a:ext cx="1143000" cy="1409700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -532,7 +591,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -568,13 +627,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1">
         <v>10</v>
-      </c>
-      <c r="E2" s="1">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="150" customHeight="1">
@@ -585,13 +644,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="150" customHeight="1">
@@ -602,13 +661,50 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="150" customHeight="1">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1">
-        <v>5</v>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="150" customHeight="1">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interface nova + Thread
</commit_message>
<xml_diff>
--- a/Estoque_Games.xlsx
+++ b/Estoque_Games.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Marca</t>
   </si>
   <si>
-    <t>Item</t>
+    <t>Jogo</t>
   </si>
   <si>
     <t>Plataforma</t>
@@ -31,49 +31,55 @@
     <t>Capa</t>
   </si>
   <si>
+    <t xml:space="preserve">Bangood </t>
+  </si>
+  <si>
     <t>Rockstar</t>
   </si>
   <si>
-    <t>dada</t>
-  </si>
-  <si>
     <t>Mojang</t>
   </si>
   <si>
-    <t>Activision</t>
+    <t>Crash bandicoot</t>
+  </si>
+  <si>
+    <t>Need For speed</t>
+  </si>
+  <si>
+    <t>Minecraft</t>
   </si>
   <si>
     <t>GTA V</t>
   </si>
   <si>
-    <t>Need For Speed</t>
-  </si>
-  <si>
-    <t>fdfd</t>
-  </si>
-  <si>
-    <t>Minecraft</t>
-  </si>
-  <si>
-    <t>Black Ops II</t>
-  </si>
-  <si>
-    <t>Xbox One</t>
+    <t>Red dead Redemption II</t>
+  </si>
+  <si>
+    <t>Red dead Redemption</t>
+  </si>
+  <si>
+    <t>PS2</t>
   </si>
   <si>
     <t>PS4</t>
   </si>
   <si>
-    <t>dfd</t>
-  </si>
-  <si>
     <t>PC</t>
   </si>
   <si>
-    <t>Xbox 360</t>
-  </si>
-  <si>
-    <t>?</t>
+    <t>PS3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
 </sst>
 </file>
@@ -162,11 +168,11 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1752600</xdr:rowOff>
+      <xdr:rowOff>1295400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="GTA V.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Crash bandicoot.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -180,7 +186,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6429375" y="438150"/>
-          <a:ext cx="1143000" cy="1562100"/>
+          <a:ext cx="1143000" cy="1104900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -204,7 +210,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="Need For Speed.jpg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Need For speed.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -231,13 +237,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>1552575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -255,7 +261,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6429375" y="6153150"/>
+          <a:off x="6429375" y="4248150"/>
           <a:ext cx="1143000" cy="1362075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -269,18 +275,18 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1600200</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1752600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="Black Ops II.jpg"/>
+        <xdr:cNvPr id="5" name="Picture 4" descr="GTA V.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -293,8 +299,84 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
+          <a:off x="6429375" y="6153150"/>
+          <a:ext cx="1143000" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1600200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Red dead Redemption II.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
           <a:off x="6429375" y="8058150"/>
           <a:ext cx="1143000" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1562100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="Red dead Redemption.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6429375" y="9963150"/>
+          <a:ext cx="1143000" cy="1371600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -591,7 +673,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -627,13 +709,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1">
-        <v>10</v>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="150" customHeight="1">
@@ -641,16 +723,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1">
-        <v>15</v>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="150" customHeight="1">
@@ -658,19 +740,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="150" customHeight="1">
@@ -678,16 +757,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="150" customHeight="1">
@@ -695,16 +774,33 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="150" customHeight="1">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1">
-        <v>10</v>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interface nova + thread Finalizada
</commit_message>
<xml_diff>
--- a/Estoque_Games.xlsx
+++ b/Estoque_Games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Marca</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Capa</t>
   </si>
   <si>
-    <t xml:space="preserve">Bangood </t>
+    <t>dasda</t>
   </si>
   <si>
     <t>Rockstar</t>
@@ -40,46 +40,61 @@
     <t>Mojang</t>
   </si>
   <si>
-    <t>Crash bandicoot</t>
-  </si>
-  <si>
-    <t>Need For speed</t>
+    <t>Riot</t>
+  </si>
+  <si>
+    <t>afsaad</t>
+  </si>
+  <si>
+    <t>Need For Speed</t>
+  </si>
+  <si>
+    <t>GTA V</t>
+  </si>
+  <si>
+    <t>Red Dead Redemption II</t>
+  </si>
+  <si>
+    <t>Red Dead Redemption</t>
   </si>
   <si>
     <t>Minecraft</t>
   </si>
   <si>
-    <t>GTA V</t>
-  </si>
-  <si>
-    <t>Red dead Redemption II</t>
-  </si>
-  <si>
-    <t>Red dead Redemption</t>
-  </si>
-  <si>
-    <t>PS2</t>
+    <t>League of Legends</t>
+  </si>
+  <si>
+    <t>dasdas</t>
+  </si>
+  <si>
+    <t>PC</t>
   </si>
   <si>
     <t>PS4</t>
   </si>
   <si>
-    <t>PC</t>
-  </si>
-  <si>
     <t>PS3</t>
   </si>
   <si>
-    <t>2</t>
+    <t xml:space="preserve">Xbox 360 </t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>19</t>
+    <t>15</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -161,62 +176,24 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1295400</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1552575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Crash bandicoot.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Need For Speed.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6429375" y="438150"/>
-          <a:ext cx="1143000" cy="1104900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1552575</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="Need For speed.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -244,11 +221,49 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1552575</xdr:rowOff>
+      <xdr:rowOff>1752600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Minecraft.jpg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="GTA V.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6429375" y="4248150"/>
+          <a:ext cx="1143000" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1600200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Red Dead Redemption II.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -261,8 +276,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6429375" y="4248150"/>
-          <a:ext cx="1143000" cy="1362075"/>
+          <a:off x="6429375" y="6153150"/>
+          <a:ext cx="1143000" cy="1409700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -275,18 +290,18 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1752600</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1562100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="GTA V.jpg"/>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Red Dead Redemption.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -299,8 +314,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6429375" y="6153150"/>
-          <a:ext cx="1143000" cy="1562100"/>
+          <a:off x="6429375" y="8058150"/>
+          <a:ext cx="1143000" cy="1371600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -313,18 +328,18 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1600200</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1552575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="Red dead Redemption II.jpg"/>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Minecraft.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -337,8 +352,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6429375" y="8058150"/>
-          <a:ext cx="1143000" cy="1409700"/>
+          <a:off x="6429375" y="9963150"/>
+          <a:ext cx="1143000" cy="1362075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -351,18 +366,18 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1562100</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1162050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="Red dead Redemption.jpg"/>
+        <xdr:cNvPr id="7" name="Picture 6" descr="League of Legends.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -375,8 +390,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6429375" y="9963150"/>
-          <a:ext cx="1143000" cy="1371600"/>
+          <a:off x="6429375" y="11868150"/>
+          <a:ext cx="1143000" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -673,7 +688,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -709,13 +724,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="150" customHeight="1">
@@ -726,13 +744,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="150" customHeight="1">
@@ -740,16 +758,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="150" customHeight="1">
@@ -760,13 +778,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="150" customHeight="1">
@@ -777,10 +795,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>21</v>
@@ -791,16 +809,33 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="150" customHeight="1">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>21</v>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionadop imagem da interface nova
</commit_message>
<xml_diff>
--- a/Estoque_Games.xlsx
+++ b/Estoque_Games.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
-  <si>
-    <t>Marca</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+  <si>
+    <t>Distribuidora</t>
   </si>
   <si>
     <t>Jogo</t>
@@ -31,67 +31,25 @@
     <t>Capa</t>
   </si>
   <si>
-    <t>dasda</t>
-  </si>
-  <si>
     <t>Rockstar</t>
   </si>
   <si>
-    <t>Mojang</t>
-  </si>
-  <si>
-    <t>Riot</t>
-  </si>
-  <si>
-    <t>afsaad</t>
-  </si>
-  <si>
-    <t>Need For Speed</t>
-  </si>
-  <si>
-    <t>GTA V</t>
-  </si>
-  <si>
-    <t>Red Dead Redemption II</t>
-  </si>
-  <si>
-    <t>Red Dead Redemption</t>
-  </si>
-  <si>
-    <t>Minecraft</t>
-  </si>
-  <si>
-    <t>League of Legends</t>
-  </si>
-  <si>
-    <t>dasdas</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>PS4</t>
-  </si>
-  <si>
-    <t>PS3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xbox 360 </t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>seu pai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gta </t>
+  </si>
+  <si>
+    <t>shxhsx</t>
+  </si>
+  <si>
+    <t>Bully</t>
+  </si>
+  <si>
+    <t>Ps4</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>?</t>
@@ -176,18 +134,18 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1552575</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1752600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Need For Speed.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Gta .jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -200,8 +158,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6429375" y="2343150"/>
-          <a:ext cx="1143000" cy="1362075"/>
+          <a:off x="6429375" y="438150"/>
+          <a:ext cx="1143000" cy="1562100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -221,11 +179,11 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>1333500</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1752600</xdr:rowOff>
+      <xdr:rowOff>1600200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="GTA V.jpg"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Bully.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -239,159 +197,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6429375" y="4248150"/>
-          <a:ext cx="1143000" cy="1562100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1600200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Red Dead Redemption II.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6429375" y="6153150"/>
           <a:ext cx="1143000" cy="1409700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1562100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="Red Dead Redemption.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6429375" y="8058150"/>
-          <a:ext cx="1143000" cy="1371600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1552575</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="Minecraft.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6429375" y="9963150"/>
-          <a:ext cx="1143000" cy="1362075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1162050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="League of Legends.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6429375" y="11868150"/>
-          <a:ext cx="1143000" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -688,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -724,16 +530,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="150" customHeight="1">
@@ -744,13 +547,16 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="150" customHeight="1">
@@ -758,84 +564,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="150" customHeight="1">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="150" customHeight="1">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="150" customHeight="1">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="150" customHeight="1">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>